<commit_message>
Additional excel time testing
</commit_message>
<xml_diff>
--- a/drivers/xlsx/testdata/datetime.xlsx
+++ b/drivers/xlsx/testdata/datetime.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilotoole/work/sq/sq/drivers/xlsx/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896A1D88-9A65-2449-A821-4456FEBC121E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70A2DCB-8669-204A-8C81-31120F098BF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66420" yWindow="17240" windowWidth="26840" windowHeight="15940" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
+    <workbookView xWindow="61360" yWindow="5280" windowWidth="33280" windowHeight="22480" activeTab="1" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="1" r:id="rId1"/>
+    <sheet name="time" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Long</t>
   </si>
@@ -43,6 +44,30 @@
   </si>
   <si>
     <t>mmmm d, yyyy</t>
+  </si>
+  <si>
+    <t>time1</t>
+  </si>
+  <si>
+    <t>3:17PM</t>
+  </si>
+  <si>
+    <t>3:17pm</t>
+  </si>
+  <si>
+    <t>time2</t>
+  </si>
+  <si>
+    <t>time3</t>
+  </si>
+  <si>
+    <t>time4</t>
+  </si>
+  <si>
+    <t>time5</t>
+  </si>
+  <si>
+    <t>time6</t>
   </si>
 </sst>
 </file>
@@ -92,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -100,6 +125,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B3BCD2-72AE-DA4C-A186-3225FCEC241C}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -466,4 +494,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB597E8-E975-1E40-ADBE-58D99090C452}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="236" zoomScaleNormal="236" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0.63680555555555551</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.63680555555555551</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.63680555555555551</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.63748842592592592</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update xlsx datetime test data
</commit_message>
<xml_diff>
--- a/drivers/xlsx/testdata/datetime.xlsx
+++ b/drivers/xlsx/testdata/datetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilotoole/work/sq/sq/drivers/xlsx/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8886F1-4B2B-8F4F-B0CC-8748DD592D82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70068C64-1F48-C34C-88CC-3C163892C77B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65020" yWindow="5020" windowWidth="42320" windowHeight="22480" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
+    <workbookView xWindow="66400" yWindow="4860" windowWidth="42320" windowHeight="22480" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="datetime" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Long</t>
   </si>
@@ -113,42 +113,18 @@
     <t>StampNano</t>
   </si>
   <si>
-    <t>1989-11-09T15:17:59-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59Z</t>
   </si>
   <si>
     <t>Thu Nov  9 15:17:59 1989</t>
   </si>
   <si>
-    <t>1989-11-09T15:17:59.123-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59.123Z</t>
   </si>
   <si>
-    <t>Thu, 09 Nov 1989 15:17:59 MST</t>
-  </si>
-  <si>
-    <t>Thu, 09 Nov 1989 15:17:59 -0700</t>
-  </si>
-  <si>
-    <t>1989-11-09T15:17:59.1234567-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59.1234567Z</t>
   </si>
   <si>
-    <t>09 Nov 89 15:17 MST</t>
-  </si>
-  <si>
-    <t>Thursday, 09-Nov-89 15:17:59 MST</t>
-  </si>
-  <si>
-    <t>Thu Nov 09 15:17:59 -0700 1989</t>
-  </si>
-  <si>
     <t>DateHourMinute</t>
   </si>
   <si>
@@ -167,7 +143,28 @@
     <t>RFC8222Z</t>
   </si>
   <si>
-    <t>Thu Nov  9 15:17:59 MST 1989</t>
+    <t>1989-11-09T15:17:59.123-00:00</t>
+  </si>
+  <si>
+    <t>Thu, 09 Nov 1989 15:17:59 UTC</t>
+  </si>
+  <si>
+    <t>Thu, 09 Nov 1989 15:17:59 +0000</t>
+  </si>
+  <si>
+    <t>09 Nov 89 15:17 UTC</t>
+  </si>
+  <si>
+    <t>09 Nov 89 15:17 +0000</t>
+  </si>
+  <si>
+    <t>Thursday, 09-Nov-89 15:17:59 UTC</t>
+  </si>
+  <si>
+    <t>Thu Nov 09 15:17:59 +0000 1989</t>
+  </si>
+  <si>
+    <t>Thu Nov  9 15:17:59 UTC 1989</t>
   </si>
 </sst>
 </file>
@@ -546,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7B6BED-64F9-C44C-A05D-EFA9B015AFB8}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,16 +576,16 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
@@ -603,16 +600,16 @@
         <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>21</v>
@@ -638,7 +635,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="10">
         <v>32821.636805555558</v>
@@ -647,40 +644,40 @@
         <v>32821.637488425928</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="10">
-        <v>32821.636805555558</v>
+        <v>41</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="P2" s="10">
         <v>32821.637488425928</v>
@@ -695,7 +692,7 @@
         <v>32821.637488425928</v>
       </c>
       <c r="T2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#307: Ingest cache (#354)
- Support for ingest cache, download cache, and progress bars.
</commit_message>
<xml_diff>
--- a/drivers/xlsx/testdata/datetime.xlsx
+++ b/drivers/xlsx/testdata/datetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilotoole/work/sq/sq/drivers/xlsx/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8886F1-4B2B-8F4F-B0CC-8748DD592D82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70068C64-1F48-C34C-88CC-3C163892C77B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65020" yWindow="5020" windowWidth="42320" windowHeight="22480" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
+    <workbookView xWindow="66400" yWindow="4860" windowWidth="42320" windowHeight="22480" xr2:uid="{0542D1C8-43BC-C044-8DC2-05F9FCD9DFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="datetime" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Long</t>
   </si>
@@ -113,42 +113,18 @@
     <t>StampNano</t>
   </si>
   <si>
-    <t>1989-11-09T15:17:59-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59Z</t>
   </si>
   <si>
     <t>Thu Nov  9 15:17:59 1989</t>
   </si>
   <si>
-    <t>1989-11-09T15:17:59.123-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59.123Z</t>
   </si>
   <si>
-    <t>Thu, 09 Nov 1989 15:17:59 MST</t>
-  </si>
-  <si>
-    <t>Thu, 09 Nov 1989 15:17:59 -0700</t>
-  </si>
-  <si>
-    <t>1989-11-09T15:17:59.1234567-07:00</t>
-  </si>
-  <si>
     <t>1989-11-09T15:17:59.1234567Z</t>
   </si>
   <si>
-    <t>09 Nov 89 15:17 MST</t>
-  </si>
-  <si>
-    <t>Thursday, 09-Nov-89 15:17:59 MST</t>
-  </si>
-  <si>
-    <t>Thu Nov 09 15:17:59 -0700 1989</t>
-  </si>
-  <si>
     <t>DateHourMinute</t>
   </si>
   <si>
@@ -167,7 +143,28 @@
     <t>RFC8222Z</t>
   </si>
   <si>
-    <t>Thu Nov  9 15:17:59 MST 1989</t>
+    <t>1989-11-09T15:17:59.123-00:00</t>
+  </si>
+  <si>
+    <t>Thu, 09 Nov 1989 15:17:59 UTC</t>
+  </si>
+  <si>
+    <t>Thu, 09 Nov 1989 15:17:59 +0000</t>
+  </si>
+  <si>
+    <t>09 Nov 89 15:17 UTC</t>
+  </si>
+  <si>
+    <t>09 Nov 89 15:17 +0000</t>
+  </si>
+  <si>
+    <t>Thursday, 09-Nov-89 15:17:59 UTC</t>
+  </si>
+  <si>
+    <t>Thu Nov 09 15:17:59 +0000 1989</t>
+  </si>
+  <si>
+    <t>Thu Nov  9 15:17:59 UTC 1989</t>
   </si>
 </sst>
 </file>
@@ -546,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7B6BED-64F9-C44C-A05D-EFA9B015AFB8}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,16 +576,16 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
@@ -603,16 +600,16 @@
         <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>21</v>
@@ -638,7 +635,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="10">
         <v>32821.636805555558</v>
@@ -647,40 +644,40 @@
         <v>32821.637488425928</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="10">
-        <v>32821.636805555558</v>
+        <v>41</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="P2" s="10">
         <v>32821.637488425928</v>
@@ -695,7 +692,7 @@
         <v>32821.637488425928</v>
       </c>
       <c r="T2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>